<commit_message>
feat: added stack to verity table
</commit_message>
<xml_diff>
--- a/Rendu_3/VerityTable.xlsx
+++ b/Rendu_3/VerityTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hearc365-my.sharepoint.com/personal/gabriel_dostuni_he-arc_ch/Documents/Documents/HeArc/ISC1b/systemes_numériques/LaboSystemNumeric/Rendu_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hearc365-my.sharepoint.com/personal/gabriel_dostuni_he-arc_ch/Documents/Documents/HeArc/ISC1b/systemes_numériques/LaboSystemNumeric/Rendu_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="519" documentId="11_AD4DB114E441178AC67DF403BE13D00A693EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59E7981F-7BEA-4B3F-9EAA-D8844795DDB4}"/>
+  <xr:revisionPtr revIDLastSave="557" documentId="11_AD4DB114E441178AC67DF403BE13D00A693EDF26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5245D700-F4CB-41F9-8719-CB3E8DEBBF74}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="64">
   <si>
     <t>opcode_i</t>
   </si>
@@ -205,6 +205,18 @@
   </si>
   <si>
     <t>TRFNC</t>
+  </si>
+  <si>
+    <t>push_pop_o (0)</t>
+  </si>
+  <si>
+    <t>push_pop_o (1)</t>
+  </si>
+  <si>
+    <t>CallFunc</t>
+  </si>
+  <si>
+    <t>ReturnFunc</t>
   </si>
 </sst>
 </file>
@@ -366,7 +378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -433,19 +445,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -465,6 +464,54 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
       <top style="thick">
         <color indexed="64"/>
       </top>
@@ -496,7 +543,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -519,16 +566,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -565,10 +621,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -834,39 +886,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O61"/>
+  <dimension ref="B1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="15" width="20.77734375" style="1" customWidth="1"/>
+    <col min="2" max="5" width="20.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="17" width="20.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1"/>
-    <row r="2" spans="2:15" ht="31.2" thickTop="1" thickBot="1">
-      <c r="B2" s="10" t="s">
+    <row r="1" spans="2:17" ht="15" thickBot="1"/>
+    <row r="2" spans="2:17" ht="31.2" thickTop="1" thickBot="1">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-    </row>
-    <row r="3" spans="2:15" ht="18.600000000000001" thickTop="1" thickBot="1">
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="14"/>
+    </row>
+    <row r="3" spans="2:17" ht="18.600000000000001" thickTop="1" thickBot="1">
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
@@ -885,32 +942,38 @@
       <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" s="4" customFormat="1" ht="15" thickTop="1">
+      <c r="P3" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" s="4" customFormat="1" ht="15" thickTop="1">
       <c r="B4" s="6">
         <v>0</v>
       </c>
@@ -950,11 +1013,17 @@
       <c r="N4" s="5">
         <v>0</v>
       </c>
-      <c r="O4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" s="4" customFormat="1">
+      <c r="O4" s="8">
+        <v>0</v>
+      </c>
+      <c r="P4" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" s="4" customFormat="1">
       <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
@@ -997,8 +1066,14 @@
       <c r="O5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" s="4" customFormat="1">
+      <c r="P5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" s="4" customFormat="1">
       <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
@@ -1041,8 +1116,14 @@
       <c r="O6" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" s="4" customFormat="1">
+      <c r="P6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" s="4" customFormat="1">
       <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1085,8 +1166,14 @@
       <c r="O7" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" s="4" customFormat="1">
+      <c r="P7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" s="4" customFormat="1">
       <c r="B8" s="5">
         <v>0</v>
       </c>
@@ -1129,8 +1216,14 @@
       <c r="O8" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:15" s="4" customFormat="1">
+      <c r="P8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" s="4" customFormat="1">
       <c r="B9" s="5">
         <v>1</v>
       </c>
@@ -1173,8 +1266,14 @@
       <c r="O9" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:15" s="4" customFormat="1">
+      <c r="P9" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" s="4" customFormat="1">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -1217,8 +1316,14 @@
       <c r="O10" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:15" s="4" customFormat="1">
+      <c r="P10" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" s="4" customFormat="1">
       <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
@@ -1261,8 +1366,14 @@
       <c r="O11" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" s="4" customFormat="1">
+      <c r="P11" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" s="4" customFormat="1">
       <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
@@ -1305,8 +1416,14 @@
       <c r="O12" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:15" s="4" customFormat="1">
+      <c r="P12" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" s="4" customFormat="1">
       <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
@@ -1349,8 +1466,14 @@
       <c r="O13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" s="4" customFormat="1">
+      <c r="P13" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" s="4" customFormat="1">
       <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
@@ -1393,8 +1516,14 @@
       <c r="O14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:15" s="4" customFormat="1">
+      <c r="P14" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" s="4" customFormat="1">
       <c r="B15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1435,8 +1564,14 @@
       <c r="O15" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="2:15" s="4" customFormat="1">
+      <c r="P15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" s="4" customFormat="1">
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1479,8 +1614,14 @@
       <c r="O16" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:15" s="4" customFormat="1">
+      <c r="P16" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" s="4" customFormat="1">
       <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
@@ -1523,8 +1664,14 @@
       <c r="O17" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:15" s="4" customFormat="1">
+      <c r="P17" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" s="4" customFormat="1">
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1567,8 +1714,14 @@
       <c r="O18" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:15" s="4" customFormat="1">
+      <c r="P18" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" s="4" customFormat="1">
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
@@ -1611,8 +1764,14 @@
       <c r="O19" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:15" s="4" customFormat="1">
+      <c r="P19" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" s="4" customFormat="1">
       <c r="B20" s="5" t="s">
         <v>17</v>
       </c>
@@ -1655,8 +1814,14 @@
       <c r="O20" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:15" s="4" customFormat="1">
+      <c r="P20" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" s="4" customFormat="1">
       <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
@@ -1699,8 +1864,14 @@
       <c r="O21" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:15" s="4" customFormat="1">
+      <c r="P21" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" s="4" customFormat="1">
       <c r="B22" s="5" t="s">
         <v>17</v>
       </c>
@@ -1743,8 +1914,14 @@
       <c r="O22" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:15" s="4" customFormat="1">
+      <c r="P22" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" s="4" customFormat="1">
       <c r="B23" s="5" t="s">
         <v>17</v>
       </c>
@@ -1787,8 +1964,14 @@
       <c r="O23" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:15" s="4" customFormat="1">
+      <c r="P23" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" s="4" customFormat="1">
       <c r="B24" s="5" t="s">
         <v>17</v>
       </c>
@@ -1831,8 +2014,14 @@
       <c r="O24" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:15" s="4" customFormat="1">
+      <c r="P24" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" s="4" customFormat="1">
       <c r="B25" s="5" t="s">
         <v>17</v>
       </c>
@@ -1875,8 +2064,14 @@
       <c r="O25" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:15" s="4" customFormat="1">
+      <c r="P25" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" s="4" customFormat="1">
       <c r="B26" s="5" t="s">
         <v>17</v>
       </c>
@@ -1919,8 +2114,14 @@
       <c r="O26" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:15" s="4" customFormat="1">
+      <c r="P26" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" s="4" customFormat="1">
       <c r="B27" s="5" t="s">
         <v>17</v>
       </c>
@@ -1963,8 +2164,14 @@
       <c r="O27" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:15" s="4" customFormat="1">
+      <c r="P27" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" s="4" customFormat="1">
       <c r="B28" s="5" t="s">
         <v>17</v>
       </c>
@@ -2007,8 +2214,14 @@
       <c r="O28" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:15" s="4" customFormat="1">
+      <c r="P28" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" s="4" customFormat="1">
       <c r="B29" s="5" t="s">
         <v>17</v>
       </c>
@@ -2051,8 +2264,14 @@
       <c r="O29" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:15" s="4" customFormat="1">
+      <c r="P29" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" s="4" customFormat="1">
       <c r="B30" s="5" t="s">
         <v>17</v>
       </c>
@@ -2095,8 +2314,14 @@
       <c r="O30" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:15" s="4" customFormat="1">
+      <c r="P30" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" s="4" customFormat="1">
       <c r="B31" s="5" t="s">
         <v>17</v>
       </c>
@@ -2139,8 +2364,14 @@
       <c r="O31" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="2:15" s="4" customFormat="1">
+      <c r="P31" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" s="4" customFormat="1">
       <c r="B32" s="5" t="s">
         <v>17</v>
       </c>
@@ -2183,8 +2414,14 @@
       <c r="O32" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="2:15" s="4" customFormat="1">
+      <c r="P32" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" s="4" customFormat="1">
       <c r="B33" s="5" t="s">
         <v>17</v>
       </c>
@@ -2227,8 +2464,14 @@
       <c r="O33" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:15" s="4" customFormat="1">
+      <c r="P33" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" s="4" customFormat="1">
       <c r="B34" s="5" t="s">
         <v>17</v>
       </c>
@@ -2271,8 +2514,14 @@
       <c r="O34" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:15" s="4" customFormat="1">
+      <c r="P34" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" s="4" customFormat="1">
       <c r="B35" s="5" t="s">
         <v>17</v>
       </c>
@@ -2315,8 +2564,14 @@
       <c r="O35" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:15" s="4" customFormat="1">
+      <c r="P35" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" s="4" customFormat="1">
       <c r="B36" s="5" t="s">
         <v>17</v>
       </c>
@@ -2359,8 +2614,14 @@
       <c r="O36" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:15" s="4" customFormat="1">
+      <c r="P36" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" s="4" customFormat="1">
       <c r="B37" s="5" t="s">
         <v>17</v>
       </c>
@@ -2403,8 +2664,14 @@
       <c r="O37" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="2:15" s="4" customFormat="1">
+      <c r="P37" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" s="4" customFormat="1">
       <c r="B38" s="5" t="s">
         <v>17</v>
       </c>
@@ -2447,8 +2714,14 @@
       <c r="O38" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:15" s="4" customFormat="1">
+      <c r="P38" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" s="4" customFormat="1">
       <c r="B39" s="5" t="s">
         <v>17</v>
       </c>
@@ -2491,8 +2764,14 @@
       <c r="O39" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:15" s="4" customFormat="1">
+      <c r="P39" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" s="4" customFormat="1">
       <c r="B40" s="5" t="s">
         <v>17</v>
       </c>
@@ -2535,8 +2814,14 @@
       <c r="O40" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:15" s="4" customFormat="1">
+      <c r="P40" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" s="4" customFormat="1">
       <c r="B41" s="5" t="s">
         <v>17</v>
       </c>
@@ -2579,8 +2864,14 @@
       <c r="O41" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="2:15" s="4" customFormat="1">
+      <c r="P41" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" s="4" customFormat="1">
       <c r="B42" s="5" t="s">
         <v>17</v>
       </c>
@@ -2623,8 +2914,14 @@
       <c r="O42" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="2:15" s="4" customFormat="1">
+      <c r="P42" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" s="4" customFormat="1">
       <c r="B43" s="5" t="s">
         <v>17</v>
       </c>
@@ -2667,8 +2964,14 @@
       <c r="O43" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="2:15" s="4" customFormat="1">
+      <c r="P43" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" s="4" customFormat="1">
       <c r="B44" s="5" t="s">
         <v>17</v>
       </c>
@@ -2711,8 +3014,14 @@
       <c r="O44" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="2:15" s="4" customFormat="1">
+      <c r="P44" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" s="4" customFormat="1">
       <c r="B45" s="5" t="s">
         <v>17</v>
       </c>
@@ -2755,8 +3064,14 @@
       <c r="O45" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="2:15" s="4" customFormat="1">
+      <c r="P45" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" s="4" customFormat="1">
       <c r="B46" s="5" t="s">
         <v>17</v>
       </c>
@@ -2799,8 +3114,14 @@
       <c r="O46" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="2:15" s="4" customFormat="1">
+      <c r="P46" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" s="4" customFormat="1">
       <c r="B47" s="5" t="s">
         <v>17</v>
       </c>
@@ -2843,8 +3164,14 @@
       <c r="O47" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="2:15" s="4" customFormat="1">
+      <c r="P47" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" s="4" customFormat="1">
       <c r="B48" s="5" t="s">
         <v>17</v>
       </c>
@@ -2887,8 +3214,14 @@
       <c r="O48" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="2:15" s="4" customFormat="1">
+      <c r="P48" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" s="4" customFormat="1">
       <c r="B49" s="5" t="s">
         <v>17</v>
       </c>
@@ -2931,8 +3264,14 @@
       <c r="O49" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="2:15" s="4" customFormat="1">
+      <c r="P49" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" s="4" customFormat="1">
       <c r="B50" s="5" t="s">
         <v>17</v>
       </c>
@@ -2975,8 +3314,14 @@
       <c r="O50" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="2:15" s="4" customFormat="1">
+      <c r="P50" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17" s="4" customFormat="1">
       <c r="B51" s="5" t="s">
         <v>17</v>
       </c>
@@ -3019,8 +3364,14 @@
       <c r="O51" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="2:15" s="4" customFormat="1">
+      <c r="P51" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:17" s="4" customFormat="1">
       <c r="B52" s="5" t="s">
         <v>17</v>
       </c>
@@ -3063,8 +3414,14 @@
       <c r="O52" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="2:15" s="4" customFormat="1">
+      <c r="P52" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17" s="4" customFormat="1">
       <c r="B53" s="5" t="s">
         <v>17</v>
       </c>
@@ -3107,8 +3464,14 @@
       <c r="O53" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="2:15" s="4" customFormat="1">
+      <c r="P53" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17" s="4" customFormat="1">
       <c r="B54" s="5" t="s">
         <v>17</v>
       </c>
@@ -3151,8 +3514,14 @@
       <c r="O54" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="2:15" s="4" customFormat="1">
+      <c r="P54" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17" s="4" customFormat="1">
       <c r="B55" s="5" t="s">
         <v>17</v>
       </c>
@@ -3195,8 +3564,14 @@
       <c r="O55" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="2:15" s="4" customFormat="1">
+      <c r="P55" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" s="4" customFormat="1">
       <c r="B56" s="5" t="s">
         <v>17</v>
       </c>
@@ -3239,8 +3614,14 @@
       <c r="O56" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="2:15" s="4" customFormat="1">
+      <c r="P56" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" s="4" customFormat="1">
       <c r="B57" s="5" t="s">
         <v>17</v>
       </c>
@@ -3283,8 +3664,14 @@
       <c r="O57" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="2:15" s="4" customFormat="1">
+      <c r="P57" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" s="4" customFormat="1">
       <c r="B58" s="5" t="s">
         <v>17</v>
       </c>
@@ -3327,8 +3714,14 @@
       <c r="O58" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="2:15" s="4" customFormat="1">
+      <c r="P58" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17" s="4" customFormat="1">
       <c r="B59" s="5" t="s">
         <v>17</v>
       </c>
@@ -3371,8 +3764,14 @@
       <c r="O59" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="2:15" s="4" customFormat="1">
+      <c r="P59" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17" s="4" customFormat="1">
       <c r="B60" s="5" t="s">
         <v>17</v>
       </c>
@@ -3415,27 +3814,117 @@
       <c r="O60" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="2:15" s="4" customFormat="1">
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
+      <c r="P60" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:17" s="4" customFormat="1">
+      <c r="B61" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H61" s="5">
+        <v>0</v>
+      </c>
+      <c r="I61" s="5">
+        <v>0</v>
+      </c>
+      <c r="J61" s="5">
+        <v>0</v>
+      </c>
+      <c r="K61" s="5">
+        <v>0</v>
+      </c>
+      <c r="L61" s="5">
+        <v>0</v>
+      </c>
+      <c r="M61" s="5">
+        <v>0</v>
+      </c>
+      <c r="N61" s="5">
+        <v>0</v>
+      </c>
+      <c r="O61" s="5">
+        <v>0</v>
+      </c>
+      <c r="P61" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q61" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:17">
+      <c r="B62" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H62" s="5">
+        <v>0</v>
+      </c>
+      <c r="I62" s="5">
+        <v>0</v>
+      </c>
+      <c r="J62" s="5">
+        <v>0</v>
+      </c>
+      <c r="K62" s="5">
+        <v>0</v>
+      </c>
+      <c r="L62" s="5">
+        <v>0</v>
+      </c>
+      <c r="M62" s="5">
+        <v>0</v>
+      </c>
+      <c r="N62" s="5">
+        <v>0</v>
+      </c>
+      <c r="O62" s="5">
+        <v>0</v>
+      </c>
+      <c r="P62" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="5">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:O2"/>
+    <mergeCell ref="H2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>